<commit_message>
added instructions for project 5
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5046B2-09BD-F942-AAB3-17297D7B534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76E892C-B0FD-2940-880D-09F2F107264A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{8E2BECA6-270F-C740-9ED5-1344B6EDB180}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="35">
   <si>
     <t>week_start</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Spring recess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2-10, 2024 </t>
   </si>
 </sst>
 </file>
@@ -509,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFD2179-9860-BE4A-AB2A-CF760AB84B2E}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1121,6 +1124,9 @@
       <c r="A40" t="s">
         <v>31</v>
       </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
       <c r="C40" s="1">
         <v>45357</v>
       </c>
@@ -1128,7 +1134,7 @@
         <v>45353</v>
       </c>
       <c r="G40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H40" t="s">
         <v>33</v>
@@ -1266,6 +1272,9 @@
       </c>
       <c r="F48" t="s">
         <v>11</v>
+      </c>
+      <c r="H48" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated topics in syllabus
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76E892C-B0FD-2940-880D-09F2F107264A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06683624-14E6-9548-B8AC-FEE2205D8609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{8E2BECA6-270F-C740-9ED5-1344B6EDB180}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="40">
   <si>
     <t>week_start</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t xml:space="preserve">March 2-10, 2024 </t>
+  </si>
+  <si>
+    <t>Sorting, Exception handling</t>
+  </si>
+  <si>
+    <t>Random Module, Data Structures (tuples)</t>
+  </si>
+  <si>
+    <t>Operators and Expressions</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>For loops, 2D lists</t>
   </si>
 </sst>
 </file>
@@ -512,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFD2179-9860-BE4A-AB2A-CF760AB84B2E}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,7 +1041,7 @@
         <v>45308</v>
       </c>
       <c r="H33" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1041,7 +1056,7 @@
       </c>
       <c r="E34" s="2"/>
       <c r="H34" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1117,7 +1132,7 @@
         <v>45350</v>
       </c>
       <c r="H39" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1186,7 +1201,7 @@
         <v>45371</v>
       </c>
       <c r="H43" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1251,7 +1266,7 @@
       </c>
       <c r="E47" s="1"/>
       <c r="H47" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated midterm grades on the schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B00AB0-9443-F446-9702-75CDBADFCB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408F871F-4CA6-8B43-B958-83A0F3A12BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33200" yWindow="260" windowWidth="30240" windowHeight="18880" xr2:uid="{8E2BECA6-270F-C740-9ED5-1344B6EDB180}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,6 +1097,12 @@
       <c r="C37" s="1">
         <v>45336</v>
       </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>45336</v>
+      </c>
       <c r="H37" t="s">
         <v>22</v>
       </c>
@@ -1109,12 +1115,6 @@
         <v>7</v>
       </c>
       <c r="C38" s="1">
-        <v>45343</v>
-      </c>
-      <c r="D38" t="s">
-        <v>2</v>
-      </c>
-      <c r="E38" s="1">
         <v>45343</v>
       </c>
       <c r="H38" t="s">
@@ -1180,12 +1180,6 @@
       <c r="C42" s="1">
         <v>45364</v>
       </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" s="1">
-        <v>45371</v>
-      </c>
       <c r="H42" t="s">
         <v>30</v>
       </c>
@@ -1214,7 +1208,12 @@
       <c r="C44" s="1">
         <v>45378</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="1">
+        <v>45378</v>
+      </c>
       <c r="H44" t="s">
         <v>26</v>
       </c>
@@ -1228,12 +1227,6 @@
       </c>
       <c r="C45" s="1">
         <v>45385</v>
-      </c>
-      <c r="D45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="1">
-        <v>45399</v>
       </c>
       <c r="H45" t="s">
         <v>28</v>
@@ -1277,6 +1270,12 @@
         <v>15</v>
       </c>
       <c r="C48" s="1">
+        <v>45406</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="1">
         <v>45406</v>
       </c>
       <c r="H48" t="s">

</xml_diff>

<commit_message>
added project 11 to menu on the left
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694924ED-D278-3545-AC8A-145AABF3DC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F668D5A9-4BF9-3942-97EA-EF361C99A6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{8E2BECA6-270F-C740-9ED5-1344B6EDB180}"/>
+    <workbookView xWindow="-2020" yWindow="880" windowWidth="16460" windowHeight="18880" xr2:uid="{8E2BECA6-270F-C740-9ED5-1344B6EDB180}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
   <si>
     <t>week_start</t>
   </si>
@@ -146,16 +146,25 @@
     <t>Sorting, Exception handling</t>
   </si>
   <si>
-    <t>Random Module, Data Structures (tuples)</t>
-  </si>
-  <si>
-    <t>Operators and Expressions</t>
-  </si>
-  <si>
-    <t>Functions</t>
-  </si>
-  <si>
-    <t>For loops, 2D lists</t>
+    <t>Python Basics (constants, variables, comments, strings, print)</t>
+  </si>
+  <si>
+    <t>Operators and Expressions, intro to functions</t>
+  </si>
+  <si>
+    <t>Functions, input from user</t>
+  </si>
+  <si>
+    <t>Control Flow (for loops), Dictionaries</t>
+  </si>
+  <si>
+    <t>Files and strings</t>
+  </si>
+  <si>
+    <t>2D lists, nested for loops</t>
+  </si>
+  <si>
+    <t>Control Flow (for loops), mutability, random</t>
   </si>
 </sst>
 </file>
@@ -527,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFD2179-9860-BE4A-AB2A-CF760AB84B2E}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1027,7 +1036,7 @@
         <v>32</v>
       </c>
       <c r="H32" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1118,7 +1127,7 @@
         <v>45343</v>
       </c>
       <c r="H38" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1167,7 +1176,7 @@
       </c>
       <c r="E41" s="1"/>
       <c r="H41" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1181,7 +1190,7 @@
         <v>45369</v>
       </c>
       <c r="H42" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1201,7 +1210,7 @@
         <v>45378</v>
       </c>
       <c r="H43" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>